<commit_message>
Load RCT / LS encrypted data
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -53,9 +53,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>system_submitter_id</t>
-  </si>
-  <si>
     <t>sys_submit_id</t>
   </si>
   <si>
@@ -149,94 +146,97 @@
     <t>qual_ok</t>
   </si>
   <si>
-    <t>a1_pid</t>
-  </si>
-  <si>
-    <t>a1_fid</t>
-  </si>
-  <si>
-    <t>a1_enrolfacility</t>
-  </si>
-  <si>
-    <t>a1_enroldate</t>
-  </si>
-  <si>
-    <t>a1_relationship</t>
-  </si>
-  <si>
-    <t>a1_name</t>
-  </si>
-  <si>
-    <t>a1_caregiver</t>
-  </si>
-  <si>
-    <t>a1_phonenb</t>
-  </si>
-  <si>
-    <t>a1_contact_success</t>
-  </si>
-  <si>
-    <t>a1_contact_a4_d_1a</t>
-  </si>
-  <si>
-    <t>a1_contact_a4_d_1b</t>
-  </si>
-  <si>
-    <t>o1_o1_1a</t>
-  </si>
-  <si>
-    <t>o1_o1_2</t>
-  </si>
-  <si>
-    <t>o1_o1_1</t>
-  </si>
-  <si>
-    <t>n1_o3_1</t>
-  </si>
-  <si>
-    <t>n1_o3_1a</t>
-  </si>
-  <si>
-    <t>n1_o3_1a_o</t>
-  </si>
-  <si>
-    <t>n1_n1_4</t>
-  </si>
-  <si>
-    <t>n1_n1_3</t>
-  </si>
-  <si>
-    <t>n1_ref_location_name</t>
-  </si>
-  <si>
-    <t>n1_n1_3o</t>
-  </si>
-  <si>
-    <t>n1_n1_2b</t>
-  </si>
-  <si>
-    <t>n1_n1_2o</t>
-  </si>
-  <si>
-    <t>n1_n1_5</t>
-  </si>
-  <si>
-    <t>n1_n1_6</t>
-  </si>
-  <si>
-    <t>n1_n1_7</t>
-  </si>
-  <si>
-    <t>n1_maxduration</t>
-  </si>
-  <si>
-    <t>n1_n1_8a</t>
-  </si>
-  <si>
-    <t>n1_n1_8</t>
-  </si>
-  <si>
-    <t>z1_qual</t>
+    <t>a1-pid</t>
+  </si>
+  <si>
+    <t>a1-fid</t>
+  </si>
+  <si>
+    <t>a1-enrolfacility</t>
+  </si>
+  <si>
+    <t>a1-enroldate</t>
+  </si>
+  <si>
+    <t>a1-relationship</t>
+  </si>
+  <si>
+    <t>a1-name</t>
+  </si>
+  <si>
+    <t>a1-caregiver</t>
+  </si>
+  <si>
+    <t>a1-phonenb</t>
+  </si>
+  <si>
+    <t>o1-o1_1a</t>
+  </si>
+  <si>
+    <t>o1-o1_2</t>
+  </si>
+  <si>
+    <t>o1-o1_1</t>
+  </si>
+  <si>
+    <t>n1-o3_1</t>
+  </si>
+  <si>
+    <t>n1-o3_1a</t>
+  </si>
+  <si>
+    <t>n1-o3_1a_o</t>
+  </si>
+  <si>
+    <t>n1-n1_4</t>
+  </si>
+  <si>
+    <t>n1-n1_3</t>
+  </si>
+  <si>
+    <t>n1-ref_location_name</t>
+  </si>
+  <si>
+    <t>n1-n1_3o</t>
+  </si>
+  <si>
+    <t>n1-n1_2b</t>
+  </si>
+  <si>
+    <t>n1-n1_2o</t>
+  </si>
+  <si>
+    <t>n1-n1_5</t>
+  </si>
+  <si>
+    <t>n1-n1_6</t>
+  </si>
+  <si>
+    <t>n1-n1_7</t>
+  </si>
+  <si>
+    <t>n1-maxduration</t>
+  </si>
+  <si>
+    <t>n1-n1_8a</t>
+  </si>
+  <si>
+    <t>n1-n1_8</t>
+  </si>
+  <si>
+    <t>z1-qual</t>
+  </si>
+  <si>
+    <t>a1-contact-success</t>
+  </si>
+  <si>
+    <t>a1-contact-a4_d_1a</t>
+  </si>
+  <si>
+    <t>a1-contact-a4_d_1b</t>
+  </si>
+  <si>
+    <t>SubmitterID</t>
   </si>
 </sst>
 </file>
@@ -595,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -619,7 +619,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -640,15 +640,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -656,39 +656,39 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>2</v>
@@ -696,135 +696,135 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>4</v>
@@ -832,66 +832,66 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Day 7 follow-up
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -71,9 +71,6 @@
     <t>phone_nb</t>
   </si>
   <si>
-    <t>hf_id</t>
-  </si>
-  <si>
     <t>hf_name</t>
   </si>
   <si>
@@ -237,6 +234,9 @@
   </si>
   <si>
     <t>SubmitterID</t>
+  </si>
+  <si>
+    <t>fid</t>
   </si>
 </sst>
 </file>
@@ -595,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -619,7 +619,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -640,7 +640,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -656,23 +656,23 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>11</v>
@@ -680,7 +680,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>13</v>
@@ -688,7 +688,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>2</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>12</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>14</v>
@@ -712,26 +712,26 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -739,92 +739,92 @@
         <v>10</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>4</v>
@@ -832,66 +832,66 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update day 7 follow-up stats
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>old</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>fid</t>
+  </si>
+  <si>
+    <t>a1-district</t>
+  </si>
+  <si>
+    <t>district</t>
   </si>
 </sst>
 </file>
@@ -593,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -664,233 +670,241 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Day 7 follow-up data export
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>old</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>district</t>
+  </si>
+  <si>
+    <t>deidentified</t>
   </si>
 </sst>
 </file>
@@ -602,309 +605,420 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix and update hospit data log
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
   <si>
     <t>old</t>
   </si>
@@ -246,6 +246,51 @@
   </si>
   <si>
     <t>deidentified</t>
+  </si>
+  <si>
+    <t>odk_ref</t>
+  </si>
+  <si>
+    <t>pid</t>
+  </si>
+  <si>
+    <t>enrolfacility</t>
+  </si>
+  <si>
+    <t>enroldate</t>
+  </si>
+  <si>
+    <t>relationship</t>
+  </si>
+  <si>
+    <t>caregiver</t>
+  </si>
+  <si>
+    <t>phonenb</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>a4_d_1a</t>
+  </si>
+  <si>
+    <t>a4_d_1b</t>
+  </si>
+  <si>
+    <t>o1_1a</t>
+  </si>
+  <si>
+    <t>n1_2o</t>
+  </si>
+  <si>
+    <t>rhf_name</t>
+  </si>
+  <si>
+    <t>n1-ref_name</t>
+  </si>
+  <si>
+    <t>ref_name</t>
   </si>
 </sst>
 </file>
@@ -602,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -613,9 +658,10 @@
     <col min="1" max="1" width="27.625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -625,8 +671,11 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -636,8 +685,11 @@
       <c r="C2" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -647,8 +699,11 @@
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -658,8 +713,11 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>69</v>
       </c>
@@ -669,8 +727,11 @@
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>39</v>
       </c>
@@ -680,8 +741,11 @@
       <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>40</v>
       </c>
@@ -691,8 +755,11 @@
       <c r="C7" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>71</v>
       </c>
@@ -702,8 +769,11 @@
       <c r="C8" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -713,8 +783,11 @@
       <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -724,8 +797,11 @@
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
@@ -735,8 +811,11 @@
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>44</v>
       </c>
@@ -746,8 +825,11 @@
       <c r="C12" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>45</v>
       </c>
@@ -757,8 +839,11 @@
       <c r="C13" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
@@ -768,8 +853,11 @@
       <c r="C14" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>66</v>
       </c>
@@ -779,8 +867,11 @@
       <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>67</v>
       </c>
@@ -790,8 +881,11 @@
       <c r="C16" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>68</v>
       </c>
@@ -801,8 +895,11 @@
       <c r="C17" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
@@ -812,8 +909,11 @@
       <c r="C18" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>47</v>
       </c>
@@ -823,8 +923,11 @@
       <c r="C19" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>48</v>
       </c>
@@ -835,7 +938,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>49</v>
       </c>
@@ -846,7 +949,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>50</v>
       </c>
@@ -857,7 +960,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>51</v>
       </c>
@@ -868,7 +971,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>52</v>
       </c>
@@ -879,7 +982,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>53</v>
       </c>
@@ -890,7 +993,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
@@ -901,29 +1004,29 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>57</v>
       </c>
@@ -934,7 +1037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>58</v>
       </c>
@@ -944,81 +1047,98 @@
       <c r="C30" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="1">
-        <v>1</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" s="1">
         <v>1</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="1">
-        <v>1</v>
-      </c>
-      <c r="C37" s="4" t="s">
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix CSV export encoding to UTF8
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -287,10 +287,10 @@
     <t>rhf_name</t>
   </si>
   <si>
-    <t>n1-ref_name</t>
-  </si>
-  <si>
-    <t>ref_name</t>
+    <t>n1-ref_hospital_name</t>
+  </si>
+  <si>
+    <t>ref_hospital_name</t>
   </si>
 </sst>
 </file>
@@ -650,7 +650,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -658,7 +658,7 @@
     <col min="1" max="1" width="27.625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Cast referral fid as a character
Fix for crash in the Kenya database
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="105">
   <si>
     <t>old</t>
   </si>
@@ -321,6 +321,24 @@
   </si>
   <si>
     <t>a1-respondent_oth</t>
+  </si>
+  <si>
+    <t>a1-contact-exist</t>
+  </si>
+  <si>
+    <t>valid_phone</t>
+  </si>
+  <si>
+    <t>exist</t>
+  </si>
+  <si>
+    <t>a1-contact-phoneoff</t>
+  </si>
+  <si>
+    <t>phone_off</t>
+  </si>
+  <si>
+    <t>phoneoff</t>
   </si>
 </sst>
 </file>
@@ -683,21 +701,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.58203125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -711,7 +729,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -725,7 +743,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -739,7 +757,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -753,7 +771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>69</v>
       </c>
@@ -767,7 +785,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>89</v>
       </c>
@@ -781,7 +799,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
@@ -795,7 +813,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
@@ -809,7 +827,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>71</v>
       </c>
@@ -823,7 +841,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>41</v>
       </c>
@@ -837,7 +855,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>42</v>
       </c>
@@ -851,7 +869,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -865,7 +883,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>44</v>
       </c>
@@ -879,7 +897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>45</v>
       </c>
@@ -893,7 +911,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>46</v>
       </c>
@@ -907,7 +925,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>66</v>
       </c>
@@ -921,330 +939,358 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D19" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="1">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="8">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="B22" s="8">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="8">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="8">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="B24" s="8">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D25" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="1">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D26" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="1">
-        <v>1</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="1">
-        <v>1</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="1">
-        <v>1</v>
-      </c>
-      <c r="C33" s="4" t="s">
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="1">
-        <v>1</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="1">
-        <v>1</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D37" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="1">
-        <v>1</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D38" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="1">
-        <v>1</v>
-      </c>
-      <c r="C37" s="4" t="s">
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="1">
-        <v>1</v>
-      </c>
-      <c r="C38" s="4" t="s">
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="1">
-        <v>1</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="1">
-        <v>1</v>
-      </c>
-      <c r="C40" s="4" t="s">
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="1">
-        <v>1</v>
-      </c>
-      <c r="C41" s="4" t="s">
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="1">
-        <v>1</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="1">
-        <v>1</v>
-      </c>
-      <c r="C43" s="4" t="s">
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor updates of the data quality report
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="125">
   <si>
     <t>old</t>
   </si>
@@ -390,6 +390,15 @@
   </si>
   <si>
     <t>qual</t>
+  </si>
+  <si>
+    <t>meta-instanceID</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t>instanceID</t>
   </si>
 </sst>
 </file>
@@ -448,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -471,6 +480,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -752,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -763,7 +790,7 @@
     <col min="1" max="1" width="27.58203125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -776,7 +803,7 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="9" t="s">
         <v>74</v>
       </c>
     </row>
@@ -790,7 +817,7 @@
       <c r="C2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="10" t="s">
         <v>8</v>
       </c>
     </row>
@@ -804,7 +831,7 @@
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -818,7 +845,7 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -832,7 +859,7 @@
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="10" t="s">
         <v>69</v>
       </c>
     </row>
@@ -846,7 +873,7 @@
       <c r="C6" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="10" t="s">
         <v>89</v>
       </c>
     </row>
@@ -860,7 +887,7 @@
       <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="10" t="s">
         <v>75</v>
       </c>
     </row>
@@ -874,7 +901,7 @@
       <c r="C8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="10" t="s">
         <v>70</v>
       </c>
     </row>
@@ -888,7 +915,7 @@
       <c r="C9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="10" t="s">
         <v>72</v>
       </c>
     </row>
@@ -902,7 +929,7 @@
       <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="10" t="s">
         <v>76</v>
       </c>
     </row>
@@ -916,7 +943,7 @@
       <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="10" t="s">
         <v>77</v>
       </c>
     </row>
@@ -930,7 +957,7 @@
       <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="10" t="s">
         <v>78</v>
       </c>
     </row>
@@ -944,7 +971,7 @@
       <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="10" t="s">
         <v>2</v>
       </c>
     </row>
@@ -958,7 +985,7 @@
       <c r="C14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="10" t="s">
         <v>79</v>
       </c>
     </row>
@@ -972,7 +999,7 @@
       <c r="C15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="10" t="s">
         <v>80</v>
       </c>
     </row>
@@ -986,7 +1013,7 @@
       <c r="C16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="10" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1000,7 +1027,7 @@
       <c r="C17" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="10" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1014,7 +1041,7 @@
       <c r="C18" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="10" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1028,7 +1055,7 @@
       <c r="C19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="10" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1042,7 +1069,7 @@
       <c r="C20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="10" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1070,7 +1097,7 @@
       <c r="C22" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="10" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1084,7 +1111,7 @@
       <c r="C23" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="10" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1098,7 +1125,7 @@
       <c r="C24" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="10" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1112,7 +1139,7 @@
       <c r="C25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1126,7 +1153,7 @@
       <c r="C26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="10" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1140,7 +1167,7 @@
       <c r="C27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="10" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1154,7 +1181,7 @@
       <c r="C28" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="10" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1168,7 +1195,7 @@
       <c r="C29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="10" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1182,7 +1209,7 @@
       <c r="C30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="10" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1196,7 +1223,7 @@
       <c r="C31" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="10" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1210,11 +1237,11 @@
       <c r="C32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>54</v>
       </c>
@@ -1224,11 +1251,11 @@
       <c r="C33" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>56</v>
       </c>
@@ -1238,11 +1265,11 @@
       <c r="C34" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>55</v>
       </c>
@@ -1252,11 +1279,11 @@
       <c r="C35" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>57</v>
       </c>
@@ -1266,11 +1293,11 @@
       <c r="C36" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>58</v>
       </c>
@@ -1280,11 +1307,11 @@
       <c r="C37" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>87</v>
       </c>
@@ -1294,11 +1321,11 @@
       <c r="C38" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>59</v>
       </c>
@@ -1308,11 +1335,11 @@
       <c r="C39" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>60</v>
       </c>
@@ -1322,11 +1349,11 @@
       <c r="C40" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>61</v>
       </c>
@@ -1336,11 +1363,11 @@
       <c r="C41" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>62</v>
       </c>
@@ -1350,11 +1377,11 @@
       <c r="C42" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>63</v>
       </c>
@@ -1364,11 +1391,11 @@
       <c r="C43" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>64</v>
       </c>
@@ -1378,11 +1405,11 @@
       <c r="C44" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="10" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>65</v>
       </c>
@@ -1392,9 +1419,27 @@
       <c r="C45" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="10" t="s">
         <v>121</v>
       </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E46" s="12"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Day 7 dictionaries
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="143">
   <si>
     <t>old</t>
   </si>
@@ -399,6 +399,60 @@
   </si>
   <si>
     <t>instanceID</t>
+  </si>
+  <si>
+    <t>n1-o3_1aa</t>
+  </si>
+  <si>
+    <t>o3_1aa</t>
+  </si>
+  <si>
+    <t>n1-o3_1b</t>
+  </si>
+  <si>
+    <t>o3_1b</t>
+  </si>
+  <si>
+    <t>n1-o3_3</t>
+  </si>
+  <si>
+    <t>care_pathway</t>
+  </si>
+  <si>
+    <t>o3_3</t>
+  </si>
+  <si>
+    <t>n1-o3_2a</t>
+  </si>
+  <si>
+    <t>other_care_yn</t>
+  </si>
+  <si>
+    <t>other_care_provider</t>
+  </si>
+  <si>
+    <t>o3_2a</t>
+  </si>
+  <si>
+    <t>rx_day7</t>
+  </si>
+  <si>
+    <t>n1-o3_2b</t>
+  </si>
+  <si>
+    <t>rx_day7_yn</t>
+  </si>
+  <si>
+    <t>o3_2b</t>
+  </si>
+  <si>
+    <t>n1-o3_2o</t>
+  </si>
+  <si>
+    <t>o3_2o</t>
+  </si>
+  <si>
+    <t>rx_day7_oth</t>
   </si>
 </sst>
 </file>
@@ -413,7 +467,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,6 +498,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -457,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -497,6 +557,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -779,21 +842,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.58203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -807,7 +870,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -821,7 +884,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -835,7 +898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -849,7 +912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>69</v>
       </c>
@@ -863,7 +926,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>89</v>
       </c>
@@ -877,7 +940,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
@@ -891,7 +954,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
@@ -905,7 +968,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>71</v>
       </c>
@@ -919,7 +982,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>41</v>
       </c>
@@ -933,7 +996,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>42</v>
       </c>
@@ -947,7 +1010,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -961,7 +1024,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>44</v>
       </c>
@@ -975,7 +1038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>45</v>
       </c>
@@ -989,7 +1052,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>46</v>
       </c>
@@ -1003,7 +1066,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>66</v>
       </c>
@@ -1017,7 +1080,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>99</v>
       </c>
@@ -1031,7 +1094,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>102</v>
       </c>
@@ -1045,7 +1108,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>67</v>
       </c>
@@ -1059,7 +1122,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>68</v>
       </c>
@@ -1073,7 +1136,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>91</v>
       </c>
@@ -1087,7 +1150,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>93</v>
       </c>
@@ -1101,7 +1164,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>97</v>
       </c>
@@ -1115,7 +1178,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>98</v>
       </c>
@@ -1129,7 +1192,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>10</v>
       </c>
@@ -1143,7 +1206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>47</v>
       </c>
@@ -1157,7 +1220,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>48</v>
       </c>
@@ -1171,7 +1234,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>49</v>
       </c>
@@ -1185,7 +1248,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>50</v>
       </c>
@@ -1199,7 +1262,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>51</v>
       </c>
@@ -1213,7 +1276,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>52</v>
       </c>
@@ -1227,7 +1290,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>53</v>
       </c>
@@ -1241,7 +1304,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>54</v>
       </c>
@@ -1255,7 +1318,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>56</v>
       </c>
@@ -1269,7 +1332,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>55</v>
       </c>
@@ -1283,7 +1346,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>57</v>
       </c>
@@ -1297,7 +1360,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>58</v>
       </c>
@@ -1311,7 +1374,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>87</v>
       </c>
@@ -1325,7 +1388,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>59</v>
       </c>
@@ -1339,7 +1402,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>60</v>
       </c>
@@ -1353,7 +1416,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>61</v>
       </c>
@@ -1367,7 +1430,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>62</v>
       </c>
@@ -1381,7 +1444,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>63</v>
       </c>
@@ -1395,7 +1458,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>64</v>
       </c>
@@ -1409,37 +1472,121 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="1">
-        <v>1</v>
-      </c>
-      <c r="C45" s="4" t="s">
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D51" s="10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B46" s="1">
-        <v>1</v>
-      </c>
-      <c r="C46" s="2" t="s">
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="D52" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="E46" s="12"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="14"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Day 7 follow-up export and duplicate review
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="146">
   <si>
     <t>old</t>
   </si>
@@ -453,6 +453,15 @@
   </si>
   <si>
     <t>rx_day7_oth</t>
+  </si>
+  <si>
+    <t>o1-o1_2a</t>
+  </si>
+  <si>
+    <t>location_death_day7</t>
+  </si>
+  <si>
+    <t>o1_2a</t>
   </si>
 </sst>
 </file>
@@ -467,7 +476,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -504,6 +513,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -517,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -560,6 +575,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -842,21 +860,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.58203125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -870,7 +888,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -884,7 +902,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -898,7 +916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -912,7 +930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>69</v>
       </c>
@@ -926,7 +944,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>89</v>
       </c>
@@ -940,7 +958,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
@@ -954,7 +972,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
@@ -968,7 +986,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>71</v>
       </c>
@@ -982,7 +1000,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>41</v>
       </c>
@@ -996,7 +1014,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>42</v>
       </c>
@@ -1010,7 +1028,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -1024,7 +1042,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>44</v>
       </c>
@@ -1038,7 +1056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>45</v>
       </c>
@@ -1052,7 +1070,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>46</v>
       </c>
@@ -1066,7 +1084,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>66</v>
       </c>
@@ -1080,7 +1098,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>99</v>
       </c>
@@ -1094,7 +1112,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>102</v>
       </c>
@@ -1108,7 +1126,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>67</v>
       </c>
@@ -1122,7 +1140,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>68</v>
       </c>
@@ -1136,7 +1154,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>91</v>
       </c>
@@ -1150,7 +1168,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>93</v>
       </c>
@@ -1164,7 +1182,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>97</v>
       </c>
@@ -1178,7 +1196,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>98</v>
       </c>
@@ -1192,7 +1210,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>10</v>
       </c>
@@ -1206,7 +1224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>47</v>
       </c>
@@ -1220,7 +1238,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>48</v>
       </c>
@@ -1234,359 +1252,373 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D29" s="10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D30" s="10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="1">
-        <v>1</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D31" s="10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="1">
-        <v>1</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D33" s="10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="1">
-        <v>1</v>
-      </c>
-      <c r="C33" s="4" t="s">
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="1">
-        <v>1</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D35" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="1">
-        <v>1</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D36" s="10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="1">
-        <v>1</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D37" s="10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="1">
-        <v>1</v>
-      </c>
-      <c r="C37" s="4" t="s">
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D38" s="10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B38" s="1">
-        <v>1</v>
-      </c>
-      <c r="C38" s="4" t="s">
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D39" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="1">
-        <v>1</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D40" s="10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="1">
-        <v>1</v>
-      </c>
-      <c r="C40" s="4" t="s">
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D41" s="10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="1">
-        <v>1</v>
-      </c>
-      <c r="C41" s="4" t="s">
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D42" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="1">
-        <v>1</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D43" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B43" s="1">
-        <v>1</v>
-      </c>
-      <c r="C43" s="4" t="s">
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D44" s="10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B44" s="1">
-        <v>1</v>
-      </c>
-      <c r="C44" s="4" t="s">
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D45" s="10" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="15" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="B45" s="1">
-        <v>1</v>
-      </c>
-      <c r="C45" s="15" t="s">
+      <c r="B46" s="1">
+        <v>1</v>
+      </c>
+      <c r="C46" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D46" s="10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="15" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="B46" s="1">
-        <v>1</v>
-      </c>
-      <c r="C46" s="15" t="s">
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+      <c r="C47" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D47" s="10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="15" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="B47" s="1">
-        <v>1</v>
-      </c>
-      <c r="C47" s="15" t="s">
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+      <c r="C48" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D48" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="15" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B48" s="1">
-        <v>1</v>
-      </c>
-      <c r="C48" s="15" t="s">
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D49" s="10" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="15" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B49" s="1">
-        <v>1</v>
-      </c>
-      <c r="C49" s="15" t="s">
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+      <c r="C50" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D50" s="10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="15" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="B50" s="1">
-        <v>1</v>
-      </c>
-      <c r="C50" s="15" t="s">
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="D51" s="10" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B51" s="1">
-        <v>1</v>
-      </c>
-      <c r="C51" s="4" t="s">
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D52" s="10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B52" s="1">
-        <v>1</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D53" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="E52" s="12"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="14"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Major refactoring of quality checks (modular)
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -862,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -904,58 +904,58 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update dictionaries for more consistency between countries
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="173">
   <si>
     <t>old</t>
   </si>
@@ -468,32 +468,108 @@
   </si>
   <si>
     <t>form_version</t>
+  </si>
+  <si>
+    <t>is_tanzania</t>
+  </si>
+  <si>
+    <t>is_india</t>
+  </si>
+  <si>
+    <t>is_kenya</t>
+  </si>
+  <si>
+    <t>is_senegal</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>a1-fu_type</t>
+  </si>
+  <si>
+    <t>fu_type</t>
+  </si>
+  <si>
+    <t>a1-call_contact-success</t>
+  </si>
+  <si>
+    <t>successful_phone_fu</t>
+  </si>
+  <si>
+    <t>a1-call_contact-exist</t>
+  </si>
+  <si>
+    <t>a1-call_contact-phoneoff</t>
+  </si>
+  <si>
+    <t>a1-call_contact-a4_d_1a</t>
+  </si>
+  <si>
+    <t>a1-a4_d_1b</t>
+  </si>
+  <si>
+    <t>a1-call_contact-first_attempt</t>
+  </si>
+  <si>
+    <t>a1-call_contact-respondent</t>
+  </si>
+  <si>
+    <t>a1-call_contact-respondent_oth</t>
+  </si>
+  <si>
+    <t>a1-physical_contact-meeting</t>
+  </si>
+  <si>
+    <t>successful_physical_fu</t>
+  </si>
+  <si>
+    <t>meeting</t>
+  </si>
+  <si>
+    <t>a1-a4_d_1a_oth</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>nominal</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>character</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -525,6 +601,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -538,59 +626,199 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -866,781 +1094,2010 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.58203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.58203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="11"/>
+    <col min="7" max="7" width="8.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="11"/>
+    <col min="9" max="9" width="9.08203125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="E1" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="E2" s="11">
+        <v>1</v>
+      </c>
+      <c r="F2" s="11">
+        <v>1</v>
+      </c>
+      <c r="G2" s="11">
+        <v>1</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="E3" s="11">
+        <v>1</v>
+      </c>
+      <c r="F3" s="11">
+        <v>1</v>
+      </c>
+      <c r="G3" s="11">
+        <v>1</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" s="11">
+        <v>1</v>
+      </c>
+      <c r="F4" s="11">
+        <v>1</v>
+      </c>
+      <c r="G4" s="11">
+        <v>1</v>
+      </c>
+      <c r="H4" s="11">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="E5" s="11">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11">
+        <v>1</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="11">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="E6" s="11">
+        <v>1</v>
+      </c>
+      <c r="F6" s="11">
+        <v>1</v>
+      </c>
+      <c r="G6" s="11">
+        <v>1</v>
+      </c>
+      <c r="H6" s="11">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D7" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="E7" s="11">
+        <v>1</v>
+      </c>
+      <c r="F7" s="11">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11">
+        <v>1</v>
+      </c>
+      <c r="H7" s="11">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D8" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="E8" s="11">
+        <v>1</v>
+      </c>
+      <c r="F8" s="11">
+        <v>1</v>
+      </c>
+      <c r="G8" s="11">
+        <v>1</v>
+      </c>
+      <c r="H8" s="11">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D9" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="E9" s="11">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11">
+        <v>1</v>
+      </c>
+      <c r="G9" s="11">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D10" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="E10" s="11">
+        <v>1</v>
+      </c>
+      <c r="F10" s="11">
+        <v>1</v>
+      </c>
+      <c r="G10" s="11">
+        <v>1</v>
+      </c>
+      <c r="H10" s="11">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D11" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="E11" s="11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B12" s="8">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="E12" s="11">
+        <v>1</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1</v>
+      </c>
+      <c r="G12" s="11">
+        <v>1</v>
+      </c>
+      <c r="H12" s="11">
+        <v>1</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D13" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="E13" s="11">
+        <v>1</v>
+      </c>
+      <c r="F13" s="11">
+        <v>1</v>
+      </c>
+      <c r="G13" s="11">
+        <v>1</v>
+      </c>
+      <c r="H13" s="11">
+        <v>1</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B14" s="8">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D14" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="E14" s="11">
+        <v>1</v>
+      </c>
+      <c r="F14" s="11">
+        <v>1</v>
+      </c>
+      <c r="G14" s="11">
+        <v>1</v>
+      </c>
+      <c r="H14" s="11">
+        <v>1</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="B15" s="8">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D15" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="E15" s="11">
+        <v>1</v>
+      </c>
+      <c r="F15" s="11">
+        <v>1</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1</v>
+      </c>
+      <c r="H15" s="11">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B16" s="8">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D16" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="E16" s="11">
+        <v>1</v>
+      </c>
+      <c r="F16" s="11">
+        <v>1</v>
+      </c>
+      <c r="G16" s="11">
+        <v>1</v>
+      </c>
+      <c r="H16" s="11">
+        <v>1</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="11">
+        <v>1</v>
+      </c>
+      <c r="F17" s="11">
+        <v>0</v>
+      </c>
+      <c r="G17" s="11">
+        <v>0</v>
+      </c>
+      <c r="H17" s="11">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="11">
+        <v>1</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0</v>
+      </c>
+      <c r="G18" s="11">
+        <v>0</v>
+      </c>
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B19" s="8">
+        <v>1</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D19" s="12" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="E19" s="11">
+        <v>0</v>
+      </c>
+      <c r="F19" s="11">
+        <v>1</v>
+      </c>
+      <c r="G19" s="11">
+        <v>1</v>
+      </c>
+      <c r="H19" s="11">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="8">
+        <v>1</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" s="11">
+        <v>1</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" s="11">
+        <v>0</v>
+      </c>
+      <c r="H20" s="11">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D21" s="12" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="E21" s="11">
+        <v>0</v>
+      </c>
+      <c r="F21" s="11">
+        <v>1</v>
+      </c>
+      <c r="G21" s="11">
+        <v>1</v>
+      </c>
+      <c r="H21" s="11">
+        <v>1</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B22" s="8">
+        <v>1</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="11">
+        <v>1</v>
+      </c>
+      <c r="F22" s="11">
+        <v>0</v>
+      </c>
+      <c r="G22" s="11">
+        <v>0</v>
+      </c>
+      <c r="H22" s="11">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="1">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D23" s="12" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="E23" s="11">
+        <v>0</v>
+      </c>
+      <c r="F23" s="11">
+        <v>1</v>
+      </c>
+      <c r="G23" s="11">
+        <v>1</v>
+      </c>
+      <c r="H23" s="11">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="8">
+        <v>1</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="11">
+        <v>1</v>
+      </c>
+      <c r="F24" s="11">
+        <v>0</v>
+      </c>
+      <c r="G24" s="11">
+        <v>0</v>
+      </c>
+      <c r="H24" s="11">
+        <v>0</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B25" s="8">
+        <v>1</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D25" s="12" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="E25" s="11">
+        <v>0</v>
+      </c>
+      <c r="F25" s="11">
+        <v>1</v>
+      </c>
+      <c r="G25" s="11">
+        <v>1</v>
+      </c>
+      <c r="H25" s="11">
+        <v>1</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="11">
+        <v>1</v>
+      </c>
+      <c r="F26" s="11">
+        <v>0</v>
+      </c>
+      <c r="G26" s="11">
+        <v>0</v>
+      </c>
+      <c r="H26" s="11">
+        <v>0</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="1">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="B27" s="8">
+        <v>1</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D27" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="E27" s="11">
+        <v>0</v>
+      </c>
+      <c r="F27" s="11">
+        <v>1</v>
+      </c>
+      <c r="G27" s="11">
+        <v>1</v>
+      </c>
+      <c r="H27" s="11">
+        <v>1</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" s="8">
+        <v>1</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="11">
+        <v>1</v>
+      </c>
+      <c r="F28" s="11">
+        <v>0</v>
+      </c>
+      <c r="G28" s="11">
+        <v>0</v>
+      </c>
+      <c r="H28" s="11">
+        <v>0</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="1">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="B29" s="8">
+        <v>1</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D29" s="12" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="E29" s="11">
+        <v>0</v>
+      </c>
+      <c r="F29" s="11">
+        <v>1</v>
+      </c>
+      <c r="G29" s="11">
+        <v>1</v>
+      </c>
+      <c r="H29" s="11">
+        <v>1</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" s="8">
+        <v>1</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="11">
+        <v>1</v>
+      </c>
+      <c r="F30" s="11">
+        <v>0</v>
+      </c>
+      <c r="G30" s="11">
+        <v>0</v>
+      </c>
+      <c r="H30" s="11">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="8">
+        <v>1</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" s="11">
+        <v>0</v>
+      </c>
+      <c r="F31" s="11">
+        <v>1</v>
+      </c>
+      <c r="G31" s="11">
+        <v>1</v>
+      </c>
+      <c r="H31" s="11">
+        <v>1</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B32" s="8">
+        <v>1</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="11">
+        <v>1</v>
+      </c>
+      <c r="F32" s="11">
+        <v>0</v>
+      </c>
+      <c r="G32" s="11">
+        <v>0</v>
+      </c>
+      <c r="H32" s="11">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="8">
+        <v>1</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="11">
+        <v>0</v>
+      </c>
+      <c r="F33" s="11">
+        <v>1</v>
+      </c>
+      <c r="G33" s="11">
+        <v>1</v>
+      </c>
+      <c r="H33" s="11">
+        <v>1</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B34" s="8">
+        <v>1</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="11">
+        <v>1</v>
+      </c>
+      <c r="F34" s="11">
+        <v>0</v>
+      </c>
+      <c r="G34" s="11">
+        <v>0</v>
+      </c>
+      <c r="H34" s="11">
+        <v>0</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="8">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="B35" s="8">
+        <v>1</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D35" s="12" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="8">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="8">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="E35" s="11">
+        <v>0</v>
+      </c>
+      <c r="F35" s="11">
+        <v>1</v>
+      </c>
+      <c r="G35" s="11">
+        <v>1</v>
+      </c>
+      <c r="H35" s="11">
+        <v>1</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" s="8">
+        <v>1</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="E36" s="11">
+        <v>1</v>
+      </c>
+      <c r="F36" s="11">
+        <v>0</v>
+      </c>
+      <c r="G36" s="11">
+        <v>0</v>
+      </c>
+      <c r="H36" s="11">
+        <v>0</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="B37" s="8">
+        <v>1</v>
+      </c>
+      <c r="C37" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D37" s="12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="E37" s="11">
+        <v>1</v>
+      </c>
+      <c r="F37" s="11">
+        <v>1</v>
+      </c>
+      <c r="G37" s="11">
+        <v>1</v>
+      </c>
+      <c r="H37" s="11">
+        <v>1</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="B38" s="8">
+        <v>1</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D38" s="13" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="E38" s="11">
+        <v>1</v>
+      </c>
+      <c r="F38" s="11">
+        <v>1</v>
+      </c>
+      <c r="G38" s="11">
+        <v>1</v>
+      </c>
+      <c r="H38" s="11">
+        <v>1</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B39" s="8">
+        <v>1</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D39" s="13" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
+      <c r="E39" s="11">
+        <v>1</v>
+      </c>
+      <c r="F39" s="11">
+        <v>1</v>
+      </c>
+      <c r="G39" s="11">
+        <v>1</v>
+      </c>
+      <c r="H39" s="11">
+        <v>1</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="15" t="s">
+      <c r="B40" s="8">
+        <v>1</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D40" s="13" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="E40" s="11">
+        <v>1</v>
+      </c>
+      <c r="F40" s="11">
+        <v>1</v>
+      </c>
+      <c r="G40" s="11">
+        <v>1</v>
+      </c>
+      <c r="H40" s="11">
+        <v>1</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B41" s="8">
+        <v>1</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D41" s="13" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="E41" s="11">
+        <v>1</v>
+      </c>
+      <c r="F41" s="11">
+        <v>1</v>
+      </c>
+      <c r="G41" s="11">
+        <v>1</v>
+      </c>
+      <c r="H41" s="11">
+        <v>1</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="1">
-        <v>1</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B42" s="8">
+        <v>1</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D42" s="14" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="E42" s="11">
+        <v>1</v>
+      </c>
+      <c r="F42" s="11">
+        <v>1</v>
+      </c>
+      <c r="G42" s="11">
+        <v>1</v>
+      </c>
+      <c r="H42" s="11">
+        <v>1</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B43" s="8">
+        <v>1</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D43" s="14" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="E43" s="11">
+        <v>1</v>
+      </c>
+      <c r="F43" s="11">
+        <v>1</v>
+      </c>
+      <c r="G43" s="11">
+        <v>1</v>
+      </c>
+      <c r="H43" s="11">
+        <v>1</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="1">
-        <v>1</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B44" s="8">
+        <v>1</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D44" s="14" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+      <c r="E44" s="11">
+        <v>1</v>
+      </c>
+      <c r="F44" s="11">
+        <v>1</v>
+      </c>
+      <c r="G44" s="11">
+        <v>1</v>
+      </c>
+      <c r="H44" s="11">
+        <v>1</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="1">
-        <v>1</v>
-      </c>
-      <c r="C33" s="4" t="s">
+      <c r="B45" s="8">
+        <v>1</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D45" s="14" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="E45" s="11">
+        <v>1</v>
+      </c>
+      <c r="F45" s="11">
+        <v>1</v>
+      </c>
+      <c r="G45" s="11">
+        <v>1</v>
+      </c>
+      <c r="H45" s="11">
+        <v>1</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="1">
-        <v>1</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="B46" s="8">
+        <v>1</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D46" s="14" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="E46" s="11">
+        <v>1</v>
+      </c>
+      <c r="F46" s="11">
+        <v>1</v>
+      </c>
+      <c r="G46" s="11">
+        <v>1</v>
+      </c>
+      <c r="H46" s="11">
+        <v>1</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="1">
-        <v>1</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="B47" s="8">
+        <v>1</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D47" s="14" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+      <c r="E47" s="11">
+        <v>1</v>
+      </c>
+      <c r="F47" s="11">
+        <v>1</v>
+      </c>
+      <c r="G47" s="11">
+        <v>1</v>
+      </c>
+      <c r="H47" s="11">
+        <v>1</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="1">
-        <v>1</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="B48" s="8">
+        <v>1</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D48" s="14" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+      <c r="E48" s="11">
+        <v>1</v>
+      </c>
+      <c r="F48" s="11">
+        <v>1</v>
+      </c>
+      <c r="G48" s="11">
+        <v>1</v>
+      </c>
+      <c r="H48" s="11">
+        <v>1</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="1">
-        <v>1</v>
-      </c>
-      <c r="C37" s="4" t="s">
+      <c r="B49" s="8">
+        <v>1</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D49" s="14" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="E49" s="11">
+        <v>1</v>
+      </c>
+      <c r="F49" s="11">
+        <v>1</v>
+      </c>
+      <c r="G49" s="11">
+        <v>1</v>
+      </c>
+      <c r="H49" s="11">
+        <v>1</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="1">
-        <v>1</v>
-      </c>
-      <c r="C38" s="4" t="s">
+      <c r="B50" s="8">
+        <v>1</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D50" s="14" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+      <c r="E50" s="11">
+        <v>1</v>
+      </c>
+      <c r="F50" s="11">
+        <v>1</v>
+      </c>
+      <c r="G50" s="11">
+        <v>1</v>
+      </c>
+      <c r="H50" s="11">
+        <v>1</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="1">
-        <v>1</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="B51" s="8">
+        <v>1</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D51" s="14" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+      <c r="E51" s="11">
+        <v>1</v>
+      </c>
+      <c r="F51" s="11">
+        <v>1</v>
+      </c>
+      <c r="G51" s="11">
+        <v>1</v>
+      </c>
+      <c r="H51" s="11">
+        <v>1</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="1">
-        <v>1</v>
-      </c>
-      <c r="C40" s="4" t="s">
+      <c r="B52" s="8">
+        <v>1</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D52" s="14" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+      <c r="E52" s="11">
+        <v>1</v>
+      </c>
+      <c r="F52" s="11">
+        <v>1</v>
+      </c>
+      <c r="G52" s="11">
+        <v>1</v>
+      </c>
+      <c r="H52" s="11">
+        <v>1</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="1">
-        <v>1</v>
-      </c>
-      <c r="C41" s="4" t="s">
+      <c r="B53" s="8">
+        <v>1</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D53" s="14" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+      <c r="E53" s="11">
+        <v>1</v>
+      </c>
+      <c r="F53" s="11">
+        <v>1</v>
+      </c>
+      <c r="G53" s="11">
+        <v>1</v>
+      </c>
+      <c r="H53" s="11">
+        <v>1</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="1">
-        <v>1</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="B54" s="8">
+        <v>1</v>
+      </c>
+      <c r="C54" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D54" s="14" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+      <c r="E54" s="11">
+        <v>1</v>
+      </c>
+      <c r="F54" s="11">
+        <v>1</v>
+      </c>
+      <c r="G54" s="11">
+        <v>1</v>
+      </c>
+      <c r="H54" s="11">
+        <v>1</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="1">
-        <v>1</v>
-      </c>
-      <c r="C43" s="4" t="s">
+      <c r="B55" s="8">
+        <v>1</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D55" s="14" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+      <c r="E55" s="11">
+        <v>1</v>
+      </c>
+      <c r="F55" s="11">
+        <v>1</v>
+      </c>
+      <c r="G55" s="11">
+        <v>1</v>
+      </c>
+      <c r="H55" s="11">
+        <v>1</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="1">
-        <v>1</v>
-      </c>
-      <c r="C44" s="4" t="s">
+      <c r="B56" s="8">
+        <v>1</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D56" s="14" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+      <c r="E56" s="11">
+        <v>1</v>
+      </c>
+      <c r="F56" s="11">
+        <v>1</v>
+      </c>
+      <c r="G56" s="11">
+        <v>1</v>
+      </c>
+      <c r="H56" s="11">
+        <v>1</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="1">
-        <v>1</v>
-      </c>
-      <c r="C45" s="4" t="s">
+      <c r="B57" s="8">
+        <v>1</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D57" s="14" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="14" t="s">
+      <c r="E57" s="11">
+        <v>1</v>
+      </c>
+      <c r="F57" s="11">
+        <v>1</v>
+      </c>
+      <c r="G57" s="11">
+        <v>1</v>
+      </c>
+      <c r="H57" s="11">
+        <v>1</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B46" s="1">
-        <v>1</v>
-      </c>
-      <c r="C46" s="14" t="s">
+      <c r="B58" s="8">
+        <v>1</v>
+      </c>
+      <c r="C58" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D58" s="14" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="14" t="s">
+      <c r="E58" s="11">
+        <v>1</v>
+      </c>
+      <c r="F58" s="11">
+        <v>1</v>
+      </c>
+      <c r="G58" s="11">
+        <v>1</v>
+      </c>
+      <c r="H58" s="11">
+        <v>1</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B47" s="1">
-        <v>1</v>
-      </c>
-      <c r="C47" s="14" t="s">
+      <c r="B59" s="8">
+        <v>1</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D59" s="14" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="14" t="s">
+      <c r="E59" s="11">
+        <v>1</v>
+      </c>
+      <c r="F59" s="11">
+        <v>1</v>
+      </c>
+      <c r="G59" s="11">
+        <v>1</v>
+      </c>
+      <c r="H59" s="11">
+        <v>1</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B48" s="1">
-        <v>1</v>
-      </c>
-      <c r="C48" s="14" t="s">
+      <c r="B60" s="8">
+        <v>1</v>
+      </c>
+      <c r="C60" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D60" s="14" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="14" t="s">
+      <c r="E60" s="11">
+        <v>1</v>
+      </c>
+      <c r="F60" s="11">
+        <v>1</v>
+      </c>
+      <c r="G60" s="11">
+        <v>1</v>
+      </c>
+      <c r="H60" s="11">
+        <v>1</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B49" s="1">
-        <v>1</v>
-      </c>
-      <c r="C49" s="14" t="s">
+      <c r="B61" s="8">
+        <v>1</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D61" s="14" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="14" t="s">
+      <c r="E61" s="11">
+        <v>1</v>
+      </c>
+      <c r="F61" s="11">
+        <v>1</v>
+      </c>
+      <c r="G61" s="11">
+        <v>1</v>
+      </c>
+      <c r="H61" s="11">
+        <v>1</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B50" s="1">
-        <v>1</v>
-      </c>
-      <c r="C50" s="14" t="s">
+      <c r="B62" s="8">
+        <v>1</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="D62" s="14" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="14" t="s">
+      <c r="E62" s="11">
+        <v>1</v>
+      </c>
+      <c r="F62" s="11">
+        <v>1</v>
+      </c>
+      <c r="G62" s="11">
+        <v>1</v>
+      </c>
+      <c r="H62" s="11">
+        <v>1</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B51" s="1">
-        <v>1</v>
-      </c>
-      <c r="C51" s="14" t="s">
+      <c r="B63" s="8">
+        <v>1</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D63" s="14" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
+      <c r="E63" s="11">
+        <v>1</v>
+      </c>
+      <c r="F63" s="11">
+        <v>1</v>
+      </c>
+      <c r="G63" s="11">
+        <v>1</v>
+      </c>
+      <c r="H63" s="11">
+        <v>1</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="1">
-        <v>1</v>
-      </c>
-      <c r="C52" s="4" t="s">
+      <c r="B64" s="8">
+        <v>1</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="D64" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="E64" s="11">
+        <v>1</v>
+      </c>
+      <c r="F64" s="11">
+        <v>1</v>
+      </c>
+      <c r="G64" s="11">
+        <v>1</v>
+      </c>
+      <c r="H64" s="11">
+        <v>1</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B53" s="1">
-        <v>1</v>
-      </c>
-      <c r="C53" s="2" t="s">
+      <c r="B65" s="8">
+        <v>1</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D65" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E53" s="11"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="13"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+      <c r="E65" s="11">
+        <v>1</v>
+      </c>
+      <c r="F65" s="11">
+        <v>1</v>
+      </c>
+      <c r="G65" s="11">
+        <v>1</v>
+      </c>
+      <c r="H65" s="11">
+        <v>1</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B54" s="1">
-        <v>1</v>
-      </c>
-      <c r="C54" s="2" t="s">
+      <c r="B66" s="8">
+        <v>1</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="D66" s="1" t="s">
         <v>146</v>
       </c>
+      <c r="E66" s="11">
+        <v>1</v>
+      </c>
+      <c r="F66" s="11">
+        <v>1</v>
+      </c>
+      <c r="G66" s="11">
+        <v>1</v>
+      </c>
+      <c r="H66" s="11">
+        <v>1</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>172</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E19:H19 E21:H21 E23:H23 E25:H25 E27:H27 E28 E29:H66 B2:B3 B5:B66">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E3 F2:H2 F3 E5:F17">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3 G5:G17">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3 H5:H17">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:F18 E20:F20 E22:F22 E24:F24 E26:F26">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18 G20 G22 G24 G26">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18 H20 H22 H24 H26">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:F4">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix incorrect logical value export from CSV
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="181">
   <si>
     <t>old</t>
   </si>
@@ -561,6 +561,12 @@
   </si>
   <si>
     <t>rhf_admission_loc_id</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>integer</t>
   </si>
 </sst>
 </file>
@@ -1174,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1188,7 +1194,7 @@
     <col min="6" max="6" width="8.6640625" style="11"/>
     <col min="7" max="7" width="8.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" style="11"/>
-    <col min="9" max="9" width="9.08203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.08203125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1250,7 +1256,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>169</v>
+        <v>8</v>
       </c>
       <c r="J2" s="11">
         <v>1</v>
@@ -1282,7 +1288,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="J3" s="11">
         <v>1</v>
@@ -1314,7 +1320,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="J4" s="11">
         <v>0</v>
@@ -1570,7 +1576,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>169</v>
+        <v>8</v>
       </c>
       <c r="J12" s="11">
         <v>0</v>
@@ -2434,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>169</v>
+        <v>8</v>
       </c>
       <c r="J39" s="11">
         <v>1</v>
@@ -2978,7 +2984,7 @@
         <v>1</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>169</v>
+        <v>8</v>
       </c>
       <c r="J56" s="11">
         <v>1</v>
@@ -3042,7 +3048,7 @@
         <v>1</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="J58" s="11">
         <v>0</v>
@@ -3106,7 +3112,7 @@
         <v>1</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="J60" s="11">
         <v>0</v>

</xml_diff>

<commit_message>
Update quality checks for Senegal and Kenya
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -440,12 +440,6 @@
     <t>o3_2b</t>
   </si>
   <si>
-    <t>n1-o3_2o</t>
-  </si>
-  <si>
-    <t>o3_2o</t>
-  </si>
-  <si>
     <t>rx_day7_oth</t>
   </si>
   <si>
@@ -570,6 +564,12 @@
   </si>
   <si>
     <t>phonenb1</t>
+  </si>
+  <si>
+    <t>n1-o3_2b_o</t>
+  </si>
+  <si>
+    <t>o3_2b_o</t>
   </si>
 </sst>
 </file>
@@ -1237,24 +1237,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.58203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.58203125" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.25" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.625" style="10"/>
-    <col min="7" max="7" width="8.125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.625" style="10"/>
+    <col min="6" max="6" width="8.58203125" style="10"/>
+    <col min="7" max="7" width="8.08203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.58203125" style="10"/>
     <col min="9" max="9" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1268,22 +1268,22 @@
         <v>73</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>149</v>
-      </c>
       <c r="I1" s="8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
@@ -1341,18 +1341,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E4" s="10">
         <v>1</v>
@@ -1370,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1428,18 +1428,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B7" s="7">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E7" s="10">
         <v>1</v>
@@ -1457,7 +1457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>70</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>44</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -1718,9 +1718,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B17" s="7">
         <v>0</v>
@@ -1729,7 +1729,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E17" s="10">
         <v>1</v>
@@ -1747,44 +1747,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="10">
+        <v>1</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0</v>
+      </c>
+      <c r="I18" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B18" s="7">
-        <v>1</v>
-      </c>
-      <c r="C18" s="11" t="s">
+      <c r="B19" s="7">
+        <v>1</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>151</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E18" s="10">
-        <v>1</v>
-      </c>
-      <c r="F18" s="10">
-        <v>0</v>
-      </c>
-      <c r="G18" s="10">
-        <v>0</v>
-      </c>
-      <c r="H18" s="10">
-        <v>0</v>
-      </c>
-      <c r="I18" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B19" s="7">
-        <v>1</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>153</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>79</v>
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>65</v>
       </c>
@@ -1834,9 +1834,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B21" s="7">
         <v>1</v>
@@ -1863,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>97</v>
       </c>
@@ -1892,9 +1892,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B23" s="7">
         <v>1</v>
@@ -1921,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>100</v>
       </c>
@@ -1950,9 +1950,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B25" s="7">
         <v>1</v>
@@ -1979,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>66</v>
       </c>
@@ -2008,9 +2008,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B27" s="7">
         <v>1</v>
@@ -2037,7 +2037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>67</v>
       </c>
@@ -2066,9 +2066,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B29" s="7">
         <v>1</v>
@@ -2095,7 +2095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>89</v>
       </c>
@@ -2118,15 +2118,15 @@
         <v>1</v>
       </c>
       <c r="H30" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B31" s="7">
         <v>1</v>
@@ -2153,7 +2153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>95</v>
       </c>
@@ -2176,15 +2176,15 @@
         <v>1</v>
       </c>
       <c r="H32" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B33" s="7">
         <v>1</v>
@@ -2211,7 +2211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>96</v>
       </c>
@@ -2240,9 +2240,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B35" s="7">
         <v>1</v>
@@ -2269,7 +2269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>91</v>
       </c>
@@ -2298,19 +2298,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B37" s="7">
+        <v>1</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="B37" s="7">
-        <v>1</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>163</v>
-      </c>
       <c r="E37" s="10">
         <v>1</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>10</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>46</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>47</v>
       </c>
@@ -2414,19 +2414,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" s="7">
+        <v>1</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D41" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="B41" s="7">
-        <v>1</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>143</v>
-      </c>
       <c r="E41" s="10">
         <v>1</v>
       </c>
@@ -2434,16 +2434,16 @@
         <v>1</v>
       </c>
       <c r="G41" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>48</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>49</v>
       </c>
@@ -2501,18 +2501,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B44" s="7">
         <v>1</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E44" s="10">
         <v>0</v>
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>50</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>51</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>52</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>53</v>
       </c>
@@ -2646,47 +2646,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="7">
+        <v>1</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D49" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="B49" s="7">
-        <v>1</v>
-      </c>
-      <c r="C49" s="5" t="s">
+      <c r="E49" s="10">
+        <v>0</v>
+      </c>
+      <c r="F49" s="10">
+        <v>1</v>
+      </c>
+      <c r="G49" s="10">
+        <v>0</v>
+      </c>
+      <c r="H49" s="10">
+        <v>0</v>
+      </c>
+      <c r="I49" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="B50" s="7">
+        <v>1</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="E49" s="10">
-        <v>0</v>
-      </c>
-      <c r="F49" s="10">
-        <v>1</v>
-      </c>
-      <c r="G49" s="10">
-        <v>0</v>
-      </c>
-      <c r="H49" s="10">
-        <v>0</v>
-      </c>
-      <c r="I49" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B50" s="7">
-        <v>1</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>174</v>
-      </c>
       <c r="D50" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E50" s="10">
         <v>0</v>
@@ -2704,7 +2704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>55</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>54</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>56</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>57</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>85</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>58</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>59</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>60</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>61</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>62</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>63</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>123</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>125</v>
       </c>
@@ -3081,19 +3081,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B64" s="7">
+        <v>1</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D64" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="B64" s="7">
-        <v>1</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="D64" s="13" t="s">
-        <v>177</v>
-      </c>
       <c r="E64" s="10">
         <v>1</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>127</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>130</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>135</v>
       </c>
@@ -3197,18 +3197,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B68" s="7">
+        <v>1</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B68" s="7">
-        <v>1</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>140</v>
-      </c>
       <c r="D68" s="13" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="E68" s="10">
         <v>1</v>
@@ -3226,7 +3226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>64</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>120</v>
       </c>
@@ -3284,18 +3284,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B71" s="7">
         <v>1</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E71" s="10">
         <v>1</v>

</xml_diff>

<commit_message>
Update Day 7 export for India
</commit_message>
<xml_diff>
--- a/inst/extdata/day7_dict.xlsx
+++ b/inst/extdata/day7_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="215">
   <si>
     <t>old</t>
   </si>
@@ -518,9 +518,6 @@
     <t>end</t>
   </si>
   <si>
-    <t>stat_analysis</t>
-  </si>
-  <si>
     <t>o3_1a_nb</t>
   </si>
   <si>
@@ -570,13 +567,115 @@
   </si>
   <si>
     <t>o3_2b_o</t>
+  </si>
+  <si>
+    <t>n1-n1_2_hvb</t>
+  </si>
+  <si>
+    <t>n1-n1_2_hhb</t>
+  </si>
+  <si>
+    <t>n1-n1_3_hvo</t>
+  </si>
+  <si>
+    <t>n1-n1_3_hho</t>
+  </si>
+  <si>
+    <t>rhf_first_loc_oth</t>
+  </si>
+  <si>
+    <t>rhf_admission_loc_oth</t>
+  </si>
+  <si>
+    <t>n1_3_hvo</t>
+  </si>
+  <si>
+    <t>n1_3_hh</t>
+  </si>
+  <si>
+    <t>n1_3_hho</t>
+  </si>
+  <si>
+    <t>rhf_first_loc_name</t>
+  </si>
+  <si>
+    <t>n1-ref_visit_location_name</t>
+  </si>
+  <si>
+    <t>ref_visit_location_name</t>
+  </si>
+  <si>
+    <t>n1-n1_2_hvo</t>
+  </si>
+  <si>
+    <t>n1-ref_visit_hospital_name</t>
+  </si>
+  <si>
+    <t>rhf_first_name</t>
+  </si>
+  <si>
+    <t>rhf_first_id</t>
+  </si>
+  <si>
+    <t>rhf_first_oth</t>
+  </si>
+  <si>
+    <t>n1_2_hvb</t>
+  </si>
+  <si>
+    <t>n1_2_hvo</t>
+  </si>
+  <si>
+    <t>date_hosp_visit_day7</t>
+  </si>
+  <si>
+    <t>n1-n1_6_hv</t>
+  </si>
+  <si>
+    <t>n1_6_hv</t>
+  </si>
+  <si>
+    <t>n1-n1_5a</t>
+  </si>
+  <si>
+    <t>n1_5a</t>
+  </si>
+  <si>
+    <t>admission_in_visit_hosp</t>
+  </si>
+  <si>
+    <t>n1-n1_2_hho</t>
+  </si>
+  <si>
+    <t>rhf_admission_id</t>
+  </si>
+  <si>
+    <t>rhf_admission_oth</t>
+  </si>
+  <si>
+    <t>n1-ref_admission_location_name</t>
+  </si>
+  <si>
+    <t>ref_admission_location_name</t>
+  </si>
+  <si>
+    <t>rhf_admission_loc_name</t>
+  </si>
+  <si>
+    <t>n1-ref_admission_hospital_name</t>
+  </si>
+  <si>
+    <t>rhf_admission_name</t>
+  </si>
+  <si>
+    <t>ref_admission_hospital_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,8 +689,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -640,6 +746,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -653,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -694,11 +806,150 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1235,26 +1486,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.58203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.58203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.25" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.58203125" style="10"/>
-    <col min="7" max="7" width="8.08203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.58203125" style="10"/>
-    <col min="9" max="9" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="10" customWidth="1"/>
+    <col min="8" max="8" width="10.75" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1279,11 +1529,8 @@
       <c r="H1" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="I1" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1308,11 +1555,8 @@
       <c r="H2" s="10">
         <v>1</v>
       </c>
-      <c r="I2" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
@@ -1337,11 +1581,8 @@
       <c r="H3" s="10">
         <v>1</v>
       </c>
-      <c r="I3" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>163</v>
       </c>
@@ -1366,11 +1607,8 @@
       <c r="H4" s="10">
         <v>1</v>
       </c>
-      <c r="I4" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1395,11 +1633,8 @@
       <c r="H5" s="10">
         <v>1</v>
       </c>
-      <c r="I5" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1424,22 +1659,19 @@
       <c r="H6" s="10">
         <v>1</v>
       </c>
-      <c r="I6" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B7" s="7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E7" s="10">
         <v>1</v>
@@ -1453,11 +1685,8 @@
       <c r="H7" s="10">
         <v>1</v>
       </c>
-      <c r="I7" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
@@ -1482,11 +1711,8 @@
       <c r="H8" s="10">
         <v>1</v>
       </c>
-      <c r="I8" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -1511,11 +1737,8 @@
       <c r="H9" s="10">
         <v>1</v>
       </c>
-      <c r="I9" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
@@ -1540,11 +1763,8 @@
       <c r="H10" s="10">
         <v>1</v>
       </c>
-      <c r="I10" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>70</v>
       </c>
@@ -1569,11 +1789,8 @@
       <c r="H11" s="10">
         <v>1</v>
       </c>
-      <c r="I11" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
@@ -1598,11 +1815,8 @@
       <c r="H12" s="10">
         <v>1</v>
       </c>
-      <c r="I12" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
@@ -1627,11 +1841,8 @@
       <c r="H13" s="10">
         <v>1</v>
       </c>
-      <c r="I13" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
@@ -1656,11 +1867,8 @@
       <c r="H14" s="10">
         <v>1</v>
       </c>
-      <c r="I14" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>44</v>
       </c>
@@ -1685,11 +1893,8 @@
       <c r="H15" s="10">
         <v>1</v>
       </c>
-      <c r="I15" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -1714,13 +1919,10 @@
       <c r="H16" s="10">
         <v>1</v>
       </c>
-      <c r="I16" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B17" s="7">
         <v>0</v>
@@ -1729,7 +1931,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E17" s="10">
         <v>1</v>
@@ -1743,11 +1945,8 @@
       <c r="H17" s="10">
         <v>1</v>
       </c>
-      <c r="I17" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>148</v>
       </c>
@@ -1772,11 +1971,8 @@
       <c r="H18" s="10">
         <v>0</v>
       </c>
-      <c r="I18" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>150</v>
       </c>
@@ -1801,11 +1997,8 @@
       <c r="H19" s="10">
         <v>0</v>
       </c>
-      <c r="I19" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>65</v>
       </c>
@@ -1830,11 +2023,8 @@
       <c r="H20" s="10">
         <v>1</v>
       </c>
-      <c r="I20" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>152</v>
       </c>
@@ -1859,11 +2049,8 @@
       <c r="H21" s="10">
         <v>0</v>
       </c>
-      <c r="I21" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>97</v>
       </c>
@@ -1888,11 +2075,8 @@
       <c r="H22" s="10">
         <v>1</v>
       </c>
-      <c r="I22" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>153</v>
       </c>
@@ -1917,11 +2101,8 @@
       <c r="H23" s="10">
         <v>0</v>
       </c>
-      <c r="I23" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>100</v>
       </c>
@@ -1946,11 +2127,8 @@
       <c r="H24" s="10">
         <v>1</v>
       </c>
-      <c r="I24" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>154</v>
       </c>
@@ -1975,11 +2153,8 @@
       <c r="H25" s="10">
         <v>0</v>
       </c>
-      <c r="I25" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>66</v>
       </c>
@@ -2004,11 +2179,8 @@
       <c r="H26" s="10">
         <v>1</v>
       </c>
-      <c r="I26" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>155</v>
       </c>
@@ -2033,11 +2205,8 @@
       <c r="H27" s="10">
         <v>0</v>
       </c>
-      <c r="I27" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>67</v>
       </c>
@@ -2062,11 +2231,8 @@
       <c r="H28" s="10">
         <v>1</v>
       </c>
-      <c r="I28" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>156</v>
       </c>
@@ -2091,11 +2257,8 @@
       <c r="H29" s="10">
         <v>0</v>
       </c>
-      <c r="I29" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>89</v>
       </c>
@@ -2120,11 +2283,8 @@
       <c r="H30" s="10">
         <v>0</v>
       </c>
-      <c r="I30" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>157</v>
       </c>
@@ -2149,11 +2309,8 @@
       <c r="H31" s="10">
         <v>0</v>
       </c>
-      <c r="I31" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>95</v>
       </c>
@@ -2178,11 +2335,8 @@
       <c r="H32" s="10">
         <v>0</v>
       </c>
-      <c r="I32" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>158</v>
       </c>
@@ -2207,11 +2361,8 @@
       <c r="H33" s="10">
         <v>0</v>
       </c>
-      <c r="I33" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>96</v>
       </c>
@@ -2236,11 +2387,8 @@
       <c r="H34" s="10">
         <v>1</v>
       </c>
-      <c r="I34" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>162</v>
       </c>
@@ -2265,11 +2413,8 @@
       <c r="H35" s="10">
         <v>0</v>
       </c>
-      <c r="I35" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>91</v>
       </c>
@@ -2294,11 +2439,8 @@
       <c r="H36" s="10">
         <v>1</v>
       </c>
-      <c r="I36" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>159</v>
       </c>
@@ -2323,11 +2465,8 @@
       <c r="H37" s="10">
         <v>0</v>
       </c>
-      <c r="I37" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>10</v>
       </c>
@@ -2352,11 +2491,8 @@
       <c r="H38" s="10">
         <v>1</v>
       </c>
-      <c r="I38" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>46</v>
       </c>
@@ -2381,11 +2517,8 @@
       <c r="H39" s="10">
         <v>1</v>
       </c>
-      <c r="I39" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>47</v>
       </c>
@@ -2410,11 +2543,8 @@
       <c r="H40" s="10">
         <v>1</v>
       </c>
-      <c r="I40" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>139</v>
       </c>
@@ -2439,11 +2569,8 @@
       <c r="H41" s="10">
         <v>0</v>
       </c>
-      <c r="I41" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>48</v>
       </c>
@@ -2468,21 +2595,18 @@
       <c r="H42" s="10">
         <v>1</v>
       </c>
-      <c r="I42" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="14" t="s">
         <v>49</v>
       </c>
       <c r="B43" s="7">
         <v>1</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="15" t="s">
         <v>105</v>
       </c>
       <c r="E43" s="10">
@@ -2497,23 +2621,20 @@
       <c r="H43" s="10">
         <v>1</v>
       </c>
-      <c r="I43" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
-        <v>167</v>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="14" t="s">
+        <v>166</v>
       </c>
       <c r="B44" s="7">
         <v>1</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D44" s="13" t="s">
+      <c r="C44" s="14" t="s">
         <v>165</v>
       </c>
+      <c r="D44" s="15" t="s">
+        <v>164</v>
+      </c>
       <c r="E44" s="10">
         <v>0</v>
       </c>
@@ -2526,21 +2647,18 @@
       <c r="H44" s="10">
         <v>0</v>
       </c>
-      <c r="I44" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="14" t="s">
         <v>50</v>
       </c>
       <c r="B45" s="7">
         <v>1</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="15" t="s">
         <v>106</v>
       </c>
       <c r="E45" s="10">
@@ -2555,21 +2673,18 @@
       <c r="H45" s="10">
         <v>1</v>
       </c>
-      <c r="I45" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="14" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="7">
         <v>1</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D46" s="15" t="s">
         <v>107</v>
       </c>
       <c r="E46" s="10">
@@ -2584,40 +2699,34 @@
       <c r="H46" s="10">
         <v>1</v>
       </c>
-      <c r="I46" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+    </row>
+    <row r="47" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="21" t="s">
         <v>52</v>
       </c>
       <c r="B47" s="7">
         <v>1</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="E47" s="10">
-        <v>1</v>
-      </c>
-      <c r="F47" s="10">
-        <v>1</v>
-      </c>
-      <c r="G47" s="10">
-        <v>1</v>
-      </c>
-      <c r="H47" s="10">
-        <v>1</v>
-      </c>
-      <c r="I47" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E47" s="23">
+        <v>1</v>
+      </c>
+      <c r="F47" s="23">
+        <v>1</v>
+      </c>
+      <c r="G47" s="23">
+        <v>1</v>
+      </c>
+      <c r="H47" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>53</v>
       </c>
@@ -2642,809 +2751,1104 @@
       <c r="H48" s="10">
         <v>1</v>
       </c>
-      <c r="I48" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="7">
+        <v>1</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="E49" s="10">
+        <v>1</v>
+      </c>
+      <c r="F49" s="10">
+        <v>1</v>
+      </c>
+      <c r="G49" s="10">
+        <v>1</v>
+      </c>
+      <c r="H49" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" s="7">
+        <v>1</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E50" s="10">
+        <v>1</v>
+      </c>
+      <c r="F50" s="10">
+        <v>1</v>
+      </c>
+      <c r="G50" s="10">
+        <v>1</v>
+      </c>
+      <c r="H50" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="7">
+        <v>1</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E51" s="10">
+        <v>1</v>
+      </c>
+      <c r="F51" s="10">
+        <v>1</v>
+      </c>
+      <c r="G51" s="10">
+        <v>1</v>
+      </c>
+      <c r="H51" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="7">
+        <v>1</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E52" s="10">
+        <v>1</v>
+      </c>
+      <c r="F52" s="10">
+        <v>1</v>
+      </c>
+      <c r="G52" s="10">
+        <v>1</v>
+      </c>
+      <c r="H52" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="7">
+        <v>1</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E53" s="10">
+        <v>1</v>
+      </c>
+      <c r="F53" s="10">
+        <v>1</v>
+      </c>
+      <c r="G53" s="10">
+        <v>1</v>
+      </c>
+      <c r="H53" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" s="7">
+        <v>1</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E54" s="10">
+        <v>1</v>
+      </c>
+      <c r="F54" s="10">
+        <v>1</v>
+      </c>
+      <c r="G54" s="10">
+        <v>1</v>
+      </c>
+      <c r="H54" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="7">
+        <v>1</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E55" s="10">
+        <v>1</v>
+      </c>
+      <c r="F55" s="10">
+        <v>1</v>
+      </c>
+      <c r="G55" s="10">
+        <v>1</v>
+      </c>
+      <c r="H55" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="7">
+        <v>1</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E56" s="10">
+        <v>1</v>
+      </c>
+      <c r="F56" s="10">
+        <v>1</v>
+      </c>
+      <c r="G56" s="10">
+        <v>1</v>
+      </c>
+      <c r="H56" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" s="7">
+        <v>1</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E57" s="10">
+        <v>1</v>
+      </c>
+      <c r="F57" s="10">
+        <v>1</v>
+      </c>
+      <c r="G57" s="10">
+        <v>1</v>
+      </c>
+      <c r="H57" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="7">
+        <v>1</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E58" s="10">
+        <v>1</v>
+      </c>
+      <c r="F58" s="10">
+        <v>1</v>
+      </c>
+      <c r="G58" s="10">
+        <v>1</v>
+      </c>
+      <c r="H58" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59" s="7">
+        <v>1</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E59" s="10">
+        <v>1</v>
+      </c>
+      <c r="F59" s="10">
+        <v>1</v>
+      </c>
+      <c r="G59" s="10">
+        <v>1</v>
+      </c>
+      <c r="H59" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B60" s="17">
+        <v>1</v>
+      </c>
+      <c r="C60" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="B49" s="7">
-        <v>1</v>
-      </c>
-      <c r="C49" s="5" t="s">
+      <c r="D60" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="E60" s="19">
+        <v>0</v>
+      </c>
+      <c r="F60" s="19">
+        <v>1</v>
+      </c>
+      <c r="G60" s="19">
+        <v>0</v>
+      </c>
+      <c r="H60" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="B61" s="17">
+        <v>1</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="E61" s="19">
+        <v>0</v>
+      </c>
+      <c r="F61" s="19">
+        <v>1</v>
+      </c>
+      <c r="G61" s="19">
+        <v>0</v>
+      </c>
+      <c r="H61" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B62" s="17">
+        <v>1</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="E62" s="19">
+        <v>0</v>
+      </c>
+      <c r="F62" s="19">
+        <v>1</v>
+      </c>
+      <c r="G62" s="19">
+        <v>0</v>
+      </c>
+      <c r="H62" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="B63" s="17">
+        <v>1</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="E63" s="19">
+        <v>0</v>
+      </c>
+      <c r="F63" s="19">
+        <v>1</v>
+      </c>
+      <c r="G63" s="19">
+        <v>0</v>
+      </c>
+      <c r="H63" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B64" s="17">
+        <v>1</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="E64" s="19">
+        <v>0</v>
+      </c>
+      <c r="F64" s="19">
+        <v>1</v>
+      </c>
+      <c r="G64" s="19">
+        <v>0</v>
+      </c>
+      <c r="H64" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B65" s="17">
+        <v>1</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="E65" s="19">
+        <v>0</v>
+      </c>
+      <c r="F65" s="19">
+        <v>1</v>
+      </c>
+      <c r="G65" s="19">
+        <v>0</v>
+      </c>
+      <c r="H65" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="B66" s="17">
+        <v>1</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E66" s="19">
+        <v>0</v>
+      </c>
+      <c r="F66" s="19">
+        <v>1</v>
+      </c>
+      <c r="G66" s="19">
+        <v>0</v>
+      </c>
+      <c r="H66" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="B67" s="17">
+        <v>1</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="E67" s="19">
+        <v>0</v>
+      </c>
+      <c r="F67" s="19">
+        <v>1</v>
+      </c>
+      <c r="G67" s="19">
+        <v>0</v>
+      </c>
+      <c r="H67" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="E49" s="10">
-        <v>0</v>
-      </c>
-      <c r="F49" s="10">
-        <v>1</v>
-      </c>
-      <c r="G49" s="10">
-        <v>0</v>
-      </c>
-      <c r="H49" s="10">
-        <v>0</v>
-      </c>
-      <c r="I49" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+      <c r="B68" s="17">
+        <v>1</v>
+      </c>
+      <c r="C68" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B50" s="7">
-        <v>1</v>
-      </c>
-      <c r="C50" s="5" t="s">
+      <c r="D68" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="E68" s="19">
+        <v>0</v>
+      </c>
+      <c r="F68" s="19">
+        <v>1</v>
+      </c>
+      <c r="G68" s="19">
+        <v>0</v>
+      </c>
+      <c r="H68" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" s="20" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="B69" s="17">
+        <v>1</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E69" s="19">
+        <v>0</v>
+      </c>
+      <c r="F69" s="19">
+        <v>1</v>
+      </c>
+      <c r="G69" s="19">
+        <v>0</v>
+      </c>
+      <c r="H69" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="B70" s="17">
+        <v>1</v>
+      </c>
+      <c r="C70" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="E70" s="19">
+        <v>0</v>
+      </c>
+      <c r="F70" s="19">
+        <v>1</v>
+      </c>
+      <c r="G70" s="19">
+        <v>0</v>
+      </c>
+      <c r="H70" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="B71" s="17">
+        <v>1</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="E71" s="19">
+        <v>0</v>
+      </c>
+      <c r="F71" s="19">
+        <v>1</v>
+      </c>
+      <c r="G71" s="19">
+        <v>0</v>
+      </c>
+      <c r="H71" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B72" s="17">
+        <v>1</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="E72" s="19">
+        <v>0</v>
+      </c>
+      <c r="F72" s="19">
+        <v>1</v>
+      </c>
+      <c r="G72" s="19">
+        <v>0</v>
+      </c>
+      <c r="H72" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B73" s="17">
+        <v>1</v>
+      </c>
+      <c r="C73" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="E73" s="19">
+        <v>0</v>
+      </c>
+      <c r="F73" s="19">
+        <v>1</v>
+      </c>
+      <c r="G73" s="19">
+        <v>0</v>
+      </c>
+      <c r="H73" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B74" s="7">
+        <v>1</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D74" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E74" s="10">
+        <v>1</v>
+      </c>
+      <c r="F74" s="10">
+        <v>1</v>
+      </c>
+      <c r="G74" s="10">
+        <v>1</v>
+      </c>
+      <c r="H74" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B75" s="7">
+        <v>1</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E75" s="10">
+        <v>1</v>
+      </c>
+      <c r="F75" s="10">
+        <v>1</v>
+      </c>
+      <c r="G75" s="10">
+        <v>1</v>
+      </c>
+      <c r="H75" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D50" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="E50" s="10">
-        <v>0</v>
-      </c>
-      <c r="F50" s="10">
-        <v>1</v>
-      </c>
-      <c r="G50" s="10">
-        <v>0</v>
-      </c>
-      <c r="H50" s="10">
-        <v>0</v>
-      </c>
-      <c r="I50" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" s="7">
-        <v>1</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="E51" s="10">
-        <v>1</v>
-      </c>
-      <c r="F51" s="10">
-        <v>1</v>
-      </c>
-      <c r="G51" s="10">
-        <v>1</v>
-      </c>
-      <c r="H51" s="10">
-        <v>1</v>
-      </c>
-      <c r="I51" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52" s="7">
-        <v>1</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E52" s="10">
-        <v>1</v>
-      </c>
-      <c r="F52" s="10">
-        <v>1</v>
-      </c>
-      <c r="G52" s="10">
-        <v>1</v>
-      </c>
-      <c r="H52" s="10">
-        <v>1</v>
-      </c>
-      <c r="I52" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="7">
-        <v>1</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E53" s="10">
-        <v>1</v>
-      </c>
-      <c r="F53" s="10">
-        <v>1</v>
-      </c>
-      <c r="G53" s="10">
-        <v>1</v>
-      </c>
-      <c r="H53" s="10">
-        <v>1</v>
-      </c>
-      <c r="I53" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B54" s="7">
-        <v>1</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E54" s="10">
-        <v>1</v>
-      </c>
-      <c r="F54" s="10">
-        <v>1</v>
-      </c>
-      <c r="G54" s="10">
-        <v>1</v>
-      </c>
-      <c r="H54" s="10">
-        <v>1</v>
-      </c>
-      <c r="I54" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B55" s="7">
-        <v>1</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E55" s="10">
-        <v>1</v>
-      </c>
-      <c r="F55" s="10">
-        <v>1</v>
-      </c>
-      <c r="G55" s="10">
-        <v>1</v>
-      </c>
-      <c r="H55" s="10">
-        <v>1</v>
-      </c>
-      <c r="I55" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" s="7">
-        <v>1</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D56" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E56" s="10">
-        <v>1</v>
-      </c>
-      <c r="F56" s="10">
-        <v>1</v>
-      </c>
-      <c r="G56" s="10">
-        <v>1</v>
-      </c>
-      <c r="H56" s="10">
-        <v>1</v>
-      </c>
-      <c r="I56" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B57" s="7">
-        <v>1</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D57" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="E57" s="10">
-        <v>1</v>
-      </c>
-      <c r="F57" s="10">
-        <v>1</v>
-      </c>
-      <c r="G57" s="10">
-        <v>1</v>
-      </c>
-      <c r="H57" s="10">
-        <v>1</v>
-      </c>
-      <c r="I57" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B58" s="7">
-        <v>1</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="E58" s="10">
-        <v>1</v>
-      </c>
-      <c r="F58" s="10">
-        <v>1</v>
-      </c>
-      <c r="G58" s="10">
-        <v>1</v>
-      </c>
-      <c r="H58" s="10">
-        <v>1</v>
-      </c>
-      <c r="I58" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B59" s="7">
-        <v>1</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="E59" s="10">
-        <v>1</v>
-      </c>
-      <c r="F59" s="10">
-        <v>1</v>
-      </c>
-      <c r="G59" s="10">
-        <v>1</v>
-      </c>
-      <c r="H59" s="10">
-        <v>1</v>
-      </c>
-      <c r="I59" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B60" s="7">
-        <v>1</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="E60" s="10">
-        <v>1</v>
-      </c>
-      <c r="F60" s="10">
-        <v>1</v>
-      </c>
-      <c r="G60" s="10">
-        <v>1</v>
-      </c>
-      <c r="H60" s="10">
-        <v>1</v>
-      </c>
-      <c r="I60" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B61" s="7">
-        <v>1</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D61" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="E61" s="10">
-        <v>1</v>
-      </c>
-      <c r="F61" s="10">
-        <v>1</v>
-      </c>
-      <c r="G61" s="10">
-        <v>1</v>
-      </c>
-      <c r="H61" s="10">
-        <v>1</v>
-      </c>
-      <c r="I61" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B62" s="7">
-        <v>1</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D62" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E62" s="10">
-        <v>1</v>
-      </c>
-      <c r="F62" s="10">
-        <v>1</v>
-      </c>
-      <c r="G62" s="10">
-        <v>1</v>
-      </c>
-      <c r="H62" s="10">
-        <v>1</v>
-      </c>
-      <c r="I62" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B63" s="7">
-        <v>1</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D63" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="E63" s="10">
-        <v>1</v>
-      </c>
-      <c r="F63" s="10">
-        <v>1</v>
-      </c>
-      <c r="G63" s="10">
-        <v>1</v>
-      </c>
-      <c r="H63" s="10">
-        <v>1</v>
-      </c>
-      <c r="I63" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
+      <c r="B76" s="7">
+        <v>1</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B64" s="7">
-        <v>1</v>
-      </c>
-      <c r="C64" s="5" t="s">
+      <c r="D76" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="D64" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="E64" s="10">
-        <v>1</v>
-      </c>
-      <c r="F64" s="10">
-        <v>1</v>
-      </c>
-      <c r="G64" s="10">
-        <v>1</v>
-      </c>
-      <c r="H64" s="10">
-        <v>1</v>
-      </c>
-      <c r="I64" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
+      <c r="E76" s="10">
+        <v>1</v>
+      </c>
+      <c r="F76" s="10">
+        <v>1</v>
+      </c>
+      <c r="G76" s="10">
+        <v>1</v>
+      </c>
+      <c r="H76" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B65" s="7">
-        <v>1</v>
-      </c>
-      <c r="C65" s="5" t="s">
+      <c r="B77" s="7">
+        <v>1</v>
+      </c>
+      <c r="C77" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D65" s="13" t="s">
+      <c r="D77" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="E65" s="10">
-        <v>1</v>
-      </c>
-      <c r="F65" s="10">
-        <v>1</v>
-      </c>
-      <c r="G65" s="10">
-        <v>1</v>
-      </c>
-      <c r="H65" s="10">
-        <v>1</v>
-      </c>
-      <c r="I65" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="5" t="s">
+      <c r="E77" s="10">
+        <v>1</v>
+      </c>
+      <c r="F77" s="10">
+        <v>1</v>
+      </c>
+      <c r="G77" s="10">
+        <v>1</v>
+      </c>
+      <c r="H77" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B66" s="7">
-        <v>1</v>
-      </c>
-      <c r="C66" s="5" t="s">
+      <c r="B78" s="7">
+        <v>1</v>
+      </c>
+      <c r="C78" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D66" s="13" t="s">
+      <c r="D78" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E66" s="10">
-        <v>1</v>
-      </c>
-      <c r="F66" s="10">
-        <v>1</v>
-      </c>
-      <c r="G66" s="10">
-        <v>1</v>
-      </c>
-      <c r="H66" s="10">
-        <v>1</v>
-      </c>
-      <c r="I66" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="5" t="s">
+      <c r="E78" s="10">
+        <v>1</v>
+      </c>
+      <c r="F78" s="10">
+        <v>1</v>
+      </c>
+      <c r="G78" s="10">
+        <v>1</v>
+      </c>
+      <c r="H78" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B67" s="7">
-        <v>1</v>
-      </c>
-      <c r="C67" s="5" t="s">
+      <c r="B79" s="7">
+        <v>1</v>
+      </c>
+      <c r="C79" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D67" s="13" t="s">
+      <c r="D79" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E67" s="10">
-        <v>1</v>
-      </c>
-      <c r="F67" s="10">
-        <v>1</v>
-      </c>
-      <c r="G67" s="10">
-        <v>1</v>
-      </c>
-      <c r="H67" s="10">
-        <v>1</v>
-      </c>
-      <c r="I67" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
+      <c r="E79" s="10">
+        <v>1</v>
+      </c>
+      <c r="F79" s="10">
+        <v>1</v>
+      </c>
+      <c r="G79" s="10">
+        <v>1</v>
+      </c>
+      <c r="H79" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B80" s="7">
+        <v>1</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D80" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="B68" s="7">
-        <v>1</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D68" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="E68" s="10">
-        <v>1</v>
-      </c>
-      <c r="F68" s="10">
-        <v>1</v>
-      </c>
-      <c r="G68" s="10">
-        <v>1</v>
-      </c>
-      <c r="H68" s="10">
-        <v>1</v>
-      </c>
-      <c r="I68" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
+      <c r="E80" s="10">
+        <v>1</v>
+      </c>
+      <c r="F80" s="10">
+        <v>1</v>
+      </c>
+      <c r="G80" s="10">
+        <v>1</v>
+      </c>
+      <c r="H80" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="7">
-        <v>1</v>
-      </c>
-      <c r="C69" s="2" t="s">
+      <c r="B81" s="7">
+        <v>1</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E69" s="10">
-        <v>1</v>
-      </c>
-      <c r="F69" s="10">
-        <v>1</v>
-      </c>
-      <c r="G69" s="10">
-        <v>1</v>
-      </c>
-      <c r="H69" s="10">
-        <v>1</v>
-      </c>
-      <c r="I69" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+      <c r="E81" s="10">
+        <v>1</v>
+      </c>
+      <c r="F81" s="10">
+        <v>1</v>
+      </c>
+      <c r="G81" s="10">
+        <v>1</v>
+      </c>
+      <c r="H81" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B70" s="7">
-        <v>1</v>
-      </c>
-      <c r="C70" s="1" t="s">
+      <c r="B82" s="7">
+        <v>1</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E70" s="10">
-        <v>1</v>
-      </c>
-      <c r="F70" s="10">
-        <v>1</v>
-      </c>
-      <c r="G70" s="10">
-        <v>1</v>
-      </c>
-      <c r="H70" s="10">
-        <v>1</v>
-      </c>
-      <c r="I70" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+      <c r="E82" s="10">
+        <v>1</v>
+      </c>
+      <c r="F82" s="10">
+        <v>1</v>
+      </c>
+      <c r="G82" s="10">
+        <v>1</v>
+      </c>
+      <c r="H82" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B71" s="7">
-        <v>1</v>
-      </c>
-      <c r="C71" s="1" t="s">
+      <c r="B83" s="7">
+        <v>1</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E71" s="10">
-        <v>1</v>
-      </c>
-      <c r="F71" s="10">
-        <v>1</v>
-      </c>
-      <c r="G71" s="10">
-        <v>1</v>
-      </c>
-      <c r="H71" s="10">
-        <v>1</v>
-      </c>
-      <c r="I71" s="10">
-        <v>0</v>
+      <c r="E83" s="10">
+        <v>1</v>
+      </c>
+      <c r="F83" s="10">
+        <v>1</v>
+      </c>
+      <c r="G83" s="10">
+        <v>1</v>
+      </c>
+      <c r="H83" s="10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E20:H20 E22:H22 E24:H24 E26:H26 E28:H28 E29 E30:H43 B2:B3 B5:B6 E45:H48 B45:B48 B51:B63 E51:H63 E65:H71 B65:B71 B8:B43">
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+  <conditionalFormatting sqref="E20:H20 E22:H22 E24:H24 E26:H26 E28:H28 E29 E30:H43 B2:B3 B5:B6 E77:H83 B77:B83 B8:B43 B74:B75 B45:B59 E74:H75 E45:H59">
+    <cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E3 F2:H2 F3 E5:F6 I2:I6 I45:I48 I51:I63 I65:I71 I8:I43 E8:F18">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+  <conditionalFormatting sqref="E2:E3 F2:H2 F3 E5:F6 E8:F18">
+    <cfRule type="cellIs" dxfId="35" priority="44" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3 G5:G6 G8:G18">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="43" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3 H5:H6 H8:H18">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="42" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:F19 E21:F21 E23:F23 E25:F25 E27:F27">
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="41" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19 G21 G23 G25 G27">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="40" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19 H21 H23 H25 H27">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="38" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="37" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="35" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:F4">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="34" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="33" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44:H44 B44">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="31" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I44">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+  <conditionalFormatting sqref="E60:H60 B60">
+    <cfRule type="cellIs" dxfId="21" priority="29" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49:H49 B49">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+  <conditionalFormatting sqref="E68:F68 B68">
+    <cfRule type="cellIs" dxfId="20" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I49">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+  <conditionalFormatting sqref="B76 E76:H76">
+    <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50:H50 B50">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+  <conditionalFormatting sqref="E7:F7">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I50">
+  <conditionalFormatting sqref="B7">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E63:H63 B63">
+    <cfRule type="cellIs" dxfId="14" priority="19" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E71:H71 B71">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E61:H61 B61 E62 G62:H62 G68:G69">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69:F69 B69 H69">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64:H64 B64">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62 F62">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B65 F65">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G65:H66 E65:E67 G67 H67:H68">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B66 F66">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B64 E64:H64">
+  <conditionalFormatting sqref="B67 F67">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I64">
+  <conditionalFormatting sqref="E72:H72 B72">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
+  <conditionalFormatting sqref="E70 G70:H70">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7:F7 I7">
+  <conditionalFormatting sqref="B70 F70">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
+  <conditionalFormatting sqref="E73 G73:H73">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="B73 F73">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>